<commit_message>
Added nodes, edges and weights. Read comments in lines 28-31. -Erick Cobo
</commit_message>
<xml_diff>
--- a/Documentos/Matriz de Adyacencia.xlsx
+++ b/Documentos/Matriz de Adyacencia.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erick Fernando Cobo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erick Fernando Cobo\PycharmProjects\Bot-Viajero\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -45,7 +45,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -55,6 +55,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -71,7 +77,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -84,6 +90,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -403,7 +412,7 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:Y26"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,116 +431,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>2</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>3</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>5</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>6</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>7</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <v>8</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="4">
         <v>9</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="4">
         <v>10</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="4">
         <v>11</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="4">
         <v>12</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="4">
         <v>13</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="4">
         <v>14</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="4">
         <v>15</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="Q2" s="4">
         <v>16</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="4">
         <v>17</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="4">
         <v>18</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="4">
         <v>19</v>
       </c>
-      <c r="U2" s="5">
+      <c r="U2" s="4">
         <v>20</v>
       </c>
-      <c r="V2" s="5">
+      <c r="V2" s="4">
         <v>21</v>
       </c>
-      <c r="W2" s="5">
+      <c r="W2" s="4">
         <v>22</v>
       </c>
-      <c r="X2" s="5">
+      <c r="X2" s="4">
         <v>23</v>
       </c>
-      <c r="Y2" s="5">
+      <c r="Y2" s="4">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="6">
         <v>0</v>
       </c>
       <c r="C3" s="1">
@@ -605,13 +614,13 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="6">
         <v>0</v>
       </c>
       <c r="D4" s="1">
@@ -682,7 +691,7 @@
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="2">
@@ -691,7 +700,7 @@
       <c r="C5" s="1">
         <v>0</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="6">
         <v>0</v>
       </c>
       <c r="E5" s="1">
@@ -759,7 +768,7 @@
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="1">
@@ -771,7 +780,7 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="6">
         <v>0</v>
       </c>
       <c r="F6" s="1">
@@ -836,7 +845,7 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="1">
@@ -851,7 +860,7 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="6">
         <v>0</v>
       </c>
       <c r="G7" s="1">
@@ -913,7 +922,7 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="1">
@@ -931,7 +940,7 @@
       <c r="F8" s="1">
         <v>0</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="6">
         <v>0</v>
       </c>
       <c r="H8" s="1">
@@ -990,7 +999,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="2">
@@ -1011,7 +1020,7 @@
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="6">
         <v>0</v>
       </c>
       <c r="I9" s="1">
@@ -1067,7 +1076,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="1">
@@ -1091,7 +1100,7 @@
       <c r="H10" s="1">
         <v>0</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="6">
         <v>0</v>
       </c>
       <c r="J10" s="1">
@@ -1144,7 +1153,7 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="2">
@@ -1171,7 +1180,7 @@
       <c r="I11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="6">
         <v>0</v>
       </c>
       <c r="K11" s="1">
@@ -1221,7 +1230,7 @@
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
       <c r="B12" s="1">
@@ -1251,7 +1260,7 @@
       <c r="J12" s="1">
         <v>0</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="6">
         <v>0</v>
       </c>
       <c r="L12" s="1">
@@ -1298,7 +1307,7 @@
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
       <c r="B13" s="1">
@@ -1331,7 +1340,7 @@
       <c r="K13" s="1">
         <v>0</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="6">
         <v>0</v>
       </c>
       <c r="M13" s="1">
@@ -1375,7 +1384,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
       <c r="B14" s="1">
@@ -1411,7 +1420,7 @@
       <c r="L14" s="1">
         <v>0</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14" s="6">
         <v>0</v>
       </c>
       <c r="N14" s="1">
@@ -1452,7 +1461,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
       <c r="B15" s="1">
@@ -1491,7 +1500,7 @@
       <c r="M15" s="1">
         <v>0</v>
       </c>
-      <c r="N15" s="1">
+      <c r="N15" s="6">
         <v>0</v>
       </c>
       <c r="O15" s="1">
@@ -1529,7 +1538,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
       <c r="B16" s="1">
@@ -1571,7 +1580,7 @@
       <c r="N16" s="1">
         <v>0</v>
       </c>
-      <c r="O16" s="1">
+      <c r="O16" s="6">
         <v>0</v>
       </c>
       <c r="P16" s="1">
@@ -1606,7 +1615,7 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
       <c r="B17" s="1">
@@ -1651,7 +1660,7 @@
       <c r="O17" s="1">
         <v>0</v>
       </c>
-      <c r="P17" s="1">
+      <c r="P17" s="6">
         <v>0</v>
       </c>
       <c r="Q17" s="1">
@@ -1683,7 +1692,7 @@
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
       <c r="B18" s="2">
@@ -1731,7 +1740,7 @@
       <c r="P18" s="1">
         <v>0</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="Q18" s="6">
         <v>0</v>
       </c>
       <c r="R18" s="1">
@@ -1760,7 +1769,7 @@
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
       <c r="B19" s="1">
@@ -1811,7 +1820,7 @@
       <c r="Q19" s="1">
         <v>0</v>
       </c>
-      <c r="R19" s="1">
+      <c r="R19" s="6">
         <v>0</v>
       </c>
       <c r="S19" s="1">
@@ -1837,7 +1846,7 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>18</v>
       </c>
       <c r="B20" s="1">
@@ -1891,7 +1900,7 @@
       <c r="R20" s="1">
         <v>0</v>
       </c>
-      <c r="S20" s="1">
+      <c r="S20" s="6">
         <v>0</v>
       </c>
       <c r="T20" s="1">
@@ -1914,7 +1923,7 @@
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="4">
         <v>19</v>
       </c>
       <c r="B21" s="1">
@@ -1971,7 +1980,7 @@
       <c r="S21" s="1">
         <v>0</v>
       </c>
-      <c r="T21" s="1">
+      <c r="T21" s="6">
         <v>0</v>
       </c>
       <c r="U21" s="1">
@@ -1991,7 +2000,7 @@
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>20</v>
       </c>
       <c r="B22" s="1">
@@ -2051,7 +2060,7 @@
       <c r="T22" s="1">
         <v>0</v>
       </c>
-      <c r="U22" s="1">
+      <c r="U22" s="6">
         <v>0</v>
       </c>
       <c r="V22" s="2">
@@ -2068,7 +2077,7 @@
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="4">
         <v>21</v>
       </c>
       <c r="B23" s="1">
@@ -2131,7 +2140,7 @@
       <c r="U23" s="2">
         <v>2.15</v>
       </c>
-      <c r="V23" s="1">
+      <c r="V23" s="6">
         <v>0</v>
       </c>
       <c r="W23" s="1">
@@ -2145,7 +2154,7 @@
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="4">
         <v>22</v>
       </c>
       <c r="B24" s="2">
@@ -2211,7 +2220,7 @@
       <c r="V24" s="1">
         <v>0</v>
       </c>
-      <c r="W24" s="1">
+      <c r="W24" s="6">
         <v>0</v>
       </c>
       <c r="X24" s="1">
@@ -2222,7 +2231,7 @@
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="4">
         <v>23</v>
       </c>
       <c r="B25" s="1">
@@ -2291,7 +2300,7 @@
       <c r="W25" s="1">
         <v>0</v>
       </c>
-      <c r="X25" s="1">
+      <c r="X25" s="6">
         <v>0</v>
       </c>
       <c r="Y25" s="1">
@@ -2299,7 +2308,7 @@
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>24</v>
       </c>
       <c r="B26" s="1">
@@ -2371,7 +2380,7 @@
       <c r="X26" s="1">
         <v>0</v>
       </c>
-      <c r="Y26" s="1">
+      <c r="Y26" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
We can now print the graph!
</commit_message>
<xml_diff>
--- a/Documentos/Matriz de Adyacencia.xlsx
+++ b/Documentos/Matriz de Adyacencia.xlsx
@@ -89,10 +89,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -412,7 +412,7 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,32 +432,32 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -540,7 +540,7 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>0</v>
       </c>
       <c r="C3" s="1">
@@ -620,7 +620,7 @@
       <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>0</v>
       </c>
       <c r="D4" s="1">
@@ -700,7 +700,7 @@
       <c r="C5" s="1">
         <v>0</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0</v>
       </c>
       <c r="E5" s="1">
@@ -780,7 +780,7 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>0</v>
       </c>
       <c r="F6" s="1">
@@ -860,7 +860,7 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>0</v>
       </c>
       <c r="G7" s="1">
@@ -940,7 +940,7 @@
       <c r="F8" s="1">
         <v>0</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>0</v>
       </c>
       <c r="H8" s="1">
@@ -1020,7 +1020,7 @@
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>0</v>
       </c>
       <c r="I9" s="1">
@@ -1100,7 +1100,7 @@
       <c r="H10" s="1">
         <v>0</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>0</v>
       </c>
       <c r="J10" s="1">
@@ -1180,7 +1180,7 @@
       <c r="I11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <v>0</v>
       </c>
       <c r="K11" s="1">
@@ -1260,7 +1260,7 @@
       <c r="J12" s="1">
         <v>0</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="5">
         <v>0</v>
       </c>
       <c r="L12" s="1">
@@ -1340,7 +1340,7 @@
       <c r="K13" s="1">
         <v>0</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="5">
         <v>0</v>
       </c>
       <c r="M13" s="1">
@@ -1420,7 +1420,7 @@
       <c r="L14" s="1">
         <v>0</v>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="5">
         <v>0</v>
       </c>
       <c r="N14" s="1">
@@ -1500,7 +1500,7 @@
       <c r="M15" s="1">
         <v>0</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="5">
         <v>0</v>
       </c>
       <c r="O15" s="1">
@@ -1580,7 +1580,7 @@
       <c r="N16" s="1">
         <v>0</v>
       </c>
-      <c r="O16" s="6">
+      <c r="O16" s="5">
         <v>0</v>
       </c>
       <c r="P16" s="1">
@@ -1660,7 +1660,7 @@
       <c r="O17" s="1">
         <v>0</v>
       </c>
-      <c r="P17" s="6">
+      <c r="P17" s="5">
         <v>0</v>
       </c>
       <c r="Q17" s="1">
@@ -1740,7 +1740,7 @@
       <c r="P18" s="1">
         <v>0</v>
       </c>
-      <c r="Q18" s="6">
+      <c r="Q18" s="5">
         <v>0</v>
       </c>
       <c r="R18" s="1">
@@ -1820,7 +1820,7 @@
       <c r="Q19" s="1">
         <v>0</v>
       </c>
-      <c r="R19" s="6">
+      <c r="R19" s="5">
         <v>0</v>
       </c>
       <c r="S19" s="1">
@@ -1900,7 +1900,7 @@
       <c r="R20" s="1">
         <v>0</v>
       </c>
-      <c r="S20" s="6">
+      <c r="S20" s="5">
         <v>0</v>
       </c>
       <c r="T20" s="1">
@@ -1980,7 +1980,7 @@
       <c r="S21" s="1">
         <v>0</v>
       </c>
-      <c r="T21" s="6">
+      <c r="T21" s="5">
         <v>0</v>
       </c>
       <c r="U21" s="1">
@@ -2060,7 +2060,7 @@
       <c r="T22" s="1">
         <v>0</v>
       </c>
-      <c r="U22" s="6">
+      <c r="U22" s="5">
         <v>0</v>
       </c>
       <c r="V22" s="2">
@@ -2140,7 +2140,7 @@
       <c r="U23" s="2">
         <v>2.15</v>
       </c>
-      <c r="V23" s="6">
+      <c r="V23" s="5">
         <v>0</v>
       </c>
       <c r="W23" s="1">
@@ -2220,7 +2220,7 @@
       <c r="V24" s="1">
         <v>0</v>
       </c>
-      <c r="W24" s="6">
+      <c r="W24" s="5">
         <v>0</v>
       </c>
       <c r="X24" s="1">
@@ -2300,7 +2300,7 @@
       <c r="W25" s="1">
         <v>0</v>
       </c>
-      <c r="X25" s="6">
+      <c r="X25" s="5">
         <v>0</v>
       </c>
       <c r="Y25" s="1">
@@ -2380,7 +2380,7 @@
       <c r="X26" s="1">
         <v>0</v>
       </c>
-      <c r="Y26" s="6">
+      <c r="Y26" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Definición de la estructura en Transportes.json
</commit_message>
<xml_diff>
--- a/Documentos/Matriz de Adyacencia.xlsx
+++ b/Documentos/Matriz de Adyacencia.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erick Fernando Cobo\PycharmProjects\Bot-Viajero\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua\Dropbox\Universidad\VI Cuatrimestre\Servicios Web\Proyectos\#2\Bot-Viajero\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,19 +24,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Pasos</t>
   </si>
   <si>
     <t>Nodos</t>
   </si>
+  <si>
+    <t>RANGOS</t>
+  </si>
+  <si>
+    <t>TAXI</t>
+  </si>
+  <si>
+    <t>0-5</t>
+  </si>
+  <si>
+    <t>BUS</t>
+  </si>
+  <si>
+    <t>0-10</t>
+  </si>
+  <si>
+    <t>TREN</t>
+  </si>
+  <si>
+    <t>5 -- 15</t>
+  </si>
+  <si>
+    <t>AVION</t>
+  </si>
+  <si>
+    <t>10 ++</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,8 +71,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -64,8 +98,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -73,11 +112,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -95,8 +150,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,16 +467,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
@@ -2390,6 +2449,44 @@
         <v>14.2</v>
       </c>
     </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:Y1"/>

</xml_diff>

<commit_message>
Agregue todos los nodos del 1 al 24 - {10,17}. Defini las relaciones. -Erick Cobo
</commit_message>
<xml_diff>
--- a/Documentos/Matriz de Adyacencia.xlsx
+++ b/Documentos/Matriz de Adyacencia.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua\Dropbox\Universidad\VI Cuatrimestre\Servicios Web\Proyectos\#2\Bot-Viajero\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erick Fernando Cobo\PycharmProjects\Bot-Viajero\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -147,11 +147,11 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -470,7 +470,7 @@
   <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,32 +491,32 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2450,40 +2450,40 @@
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="7"/>
+      <c r="B31" s="6"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>